<commit_message>
Added some non functional requirements
</commit_message>
<xml_diff>
--- a/documentation/krofulisti.xlsx
+++ b/documentation/krofulisti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D6B4CF-9689-4C79-A458-3AE3D990020A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD172F18-8625-48B2-B88B-C90041A904F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8964" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="kröfur" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="69">
   <si>
     <t>Number</t>
   </si>
@@ -191,6 +191,62 @@
   </si>
   <si>
     <t>Það þarf að vera hægt að skrá starfsmenn á hverja vinnuferð,  a.m.k. tvo flugmenn og einn þeirra er flugstjóri, a.m.k. einn flugþjón og einn þeirra er yfirflugþjónn</t>
+  </si>
+  <si>
+    <t>Non-Functional Requirements:</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta skráð nýjan starfmann í kerfið</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta skráð nýjan starfmann í 
+kerfið á innan við 2 mínútum að meðaltali</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta skráð nýja vinnuferð í kerfið</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta skráð nýja vinnuferð í kerfið
+á innan við 2 mínútum að meðaltali</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta skráð nýja flugleið í kerfið</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta látið tiltekna vinnuferð 
+endurtaka sig</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta birt lista af öllum starfsmönnum</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta birt lista af öllum starfsmönnum
+á innan við 30 sekúndum</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta látið tiltekna vinnuferð 
+endurtaka sig á innan við 2 mínútum</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að breytt upplýsingum um starfsmann</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að breytt upplýsingum um starfsmann
+á innan við 2 mínútum</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta birt lista af öllum flugleiðum</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta birt lista af öllum flugleiðum
+á innan við 30 sekúndum</t>
+  </si>
+  <si>
+    <t>Yfir 94%  skipuleggjara eiga að geta skráð nýja flugvél í kerfið</t>
+  </si>
+  <si>
+    <t>Yfir 94%  skipuleggjara eiga að geta skráð nýja flugvél í kerfið
+á innin við 2 mínútum</t>
   </si>
 </sst>
 </file>
@@ -344,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -415,6 +471,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,10 +804,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:F41"/>
+  <dimension ref="B2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1343,6 +1414,394 @@
         <v>46</v>
       </c>
       <c r="F41" s="11"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="20"/>
+      <c r="C42" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="22"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="24"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="6">
+        <v>39</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="25"/>
+    </row>
+    <row r="44" spans="2:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="6">
+        <v>40</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="25"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="6">
+        <v>41</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="25"/>
+    </row>
+    <row r="46" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B46" s="6">
+        <v>42</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" s="25"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="6">
+        <v>43</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" s="25"/>
+    </row>
+    <row r="48" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="6">
+        <v>44</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="25"/>
+    </row>
+    <row r="49" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="6">
+        <v>45</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" s="25"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="6">
+        <v>46</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="25"/>
+    </row>
+    <row r="51" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B51" s="6">
+        <v>47</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" s="25"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="6">
+        <v>48</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" s="25"/>
+    </row>
+    <row r="53" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="6">
+        <v>49</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="25"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="6">
+        <v>50</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="25"/>
+    </row>
+    <row r="55" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B55" s="6">
+        <v>51</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="25"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="6">
+        <v>52</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="25"/>
+    </row>
+    <row r="57" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B57" s="6">
+        <v>53</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="25"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="6"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="25"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="6"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="25"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="6"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="25"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="6"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="25"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="6"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="25"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="6"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="25"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B64" s="6"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="25"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65" s="6"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="25"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="6"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="25"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67" s="6"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="25"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B68" s="6"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="25"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B69" s="6"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="25"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B70" s="6"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="25"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" s="6"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="25"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="6"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="25"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B73" s="6"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="25"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74" s="6"/>
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="25"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75" s="6"/>
+      <c r="C75" s="25"/>
+      <c r="D75" s="25"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="25"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" s="6"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="25"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" s="6"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="25"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B78" s="6"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="25"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" s="26"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="27"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished the requirement list
</commit_message>
<xml_diff>
--- a/documentation/krofulisti.xlsx
+++ b/documentation/krofulisti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patti\Desktop\Verk nám\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD172F18-8625-48B2-B88B-C90041A904F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE12FF25-1498-4CF7-A7CE-93856854CC4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8964" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
+    <workbookView xWindow="-560" yWindow="710" windowWidth="13820" windowHeight="6000" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="kröfur" sheetId="2" r:id="rId1"/>
@@ -32,14 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="96">
   <si>
     <t>Number</t>
   </si>
   <si>
-    <t>user group(s)</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -61,12 +58,6 @@
     <t>Mannari</t>
   </si>
   <si>
-    <t>það þarf að vera hægt að skrá vinnuferð með áfangastað, dagsetningu og tíma brottfarar frá Íslandi, dagsetningu og tíma brottfarar til Íslands</t>
-  </si>
-  <si>
-    <t>Það þarf að vera hægt að endurtaka skráningu vinnuferðar fyrir sama áfangastað og sama tíma yfir á marga daga</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að endurtaka skráningu vinnuferðar sem viðburð sem gerist með reglulegu millibili</t>
   </si>
   <si>
@@ -82,9 +73,6 @@
     <t>Það þarf að vera hægt að sjá upplýsingar um ákveðinn starfsmann</t>
   </si>
   <si>
-    <t>Það þarf að vera hægt að breyta upplýsingum um ákveðinn starfsmann, að undanskildu nafni og kennitölu</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að sjá lista yfir alla áfangastaði</t>
   </si>
   <si>
@@ -94,9 +82,6 @@
     <t>Skipuleggjari</t>
   </si>
   <si>
-    <t>Skipuleggjari og Mannari</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að skrá vinnuferð án starfsmannaupplýsinga</t>
   </si>
   <si>
@@ -130,9 +115,6 @@
     <t>Það þarf að vera hægt að skrá flugvél á vinnuferð áður en starfsmenn eru skráðir</t>
   </si>
   <si>
-    <t>Það þarf að vera hægt að skrá áfangastað með landi, flugvelli, einkennisnúmer flugvallar, flugtíma og fjarlægð frá Íslandi ásamt nafni tengiliðs og neyðarsímanúmeri</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að sjá dagsetningu og tíma þegar flugvél er aftur laus ef hún er í notkun</t>
   </si>
   <si>
@@ -151,9 +133,6 @@
     <t>Það þarf að vera hægt að sjá lista yfir alla vinnuferðir með fjölda lausra- og seldra sæta</t>
   </si>
   <si>
-    <t>Það þarf að vera hægt að sjá lista yfir alla vinnuferðir með flugnúmerum beggja flugferðanna</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að sjá lista yfir alla flugmenn og hvaða flugvélategundum þeir mega fljúga</t>
   </si>
   <si>
@@ -187,9 +166,6 @@
     <t xml:space="preserve">Það þarf að vera hægt að skrá tvö flugnúmer á vinnuferð </t>
   </si>
   <si>
-    <t>Það þarf að vera hægt að skrá starfsmann með nafni, kennitölu, starfsheiti, heimilsfangi, heimasími, gsm-síma og netfangi</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að skrá starfsmenn á hverja vinnuferð,  a.m.k. tvo flugmenn og einn þeirra er flugstjóri, a.m.k. einn flugþjón og einn þeirra er yfirflugþjónn</t>
   </si>
   <si>
@@ -199,15 +175,7 @@
     <t>Yfir 94% mannara eiga að geta skráð nýjan starfmann í kerfið</t>
   </si>
   <si>
-    <t>Yfir 94% mannara eiga að geta skráð nýjan starfmann í 
-kerfið á innan við 2 mínútum að meðaltali</t>
-  </si>
-  <si>
     <t>Yfir 94% skipuleggjara eiga að geta skráð nýja vinnuferð í kerfið</t>
-  </si>
-  <si>
-    <t>Yfir 94% skipuleggjara eiga að geta skráð nýja vinnuferð í kerfið
-á innan við 2 mínútum að meðaltali</t>
   </si>
   <si>
     <t>Yfir 94% skipuleggjara eiga að geta skráð nýja flugleið í kerfið</t>
@@ -220,10 +188,6 @@
     <t>Yfir 94% mannara eiga að geta birt lista af öllum starfsmönnum</t>
   </si>
   <si>
-    <t>Yfir 94% mannara eiga að geta birt lista af öllum starfsmönnum
-á innan við 30 sekúndum</t>
-  </si>
-  <si>
     <t>Yfir 94% skipuleggjara eiga að geta látið tiltekna vinnuferð 
 endurtaka sig á innan við 2 mínútum</t>
   </si>
@@ -231,22 +195,154 @@
     <t>Yfir 94% mannara eiga að breytt upplýsingum um starfsmann</t>
   </si>
   <si>
+    <t>Yfir 94% skipuleggjara eiga að geta birt lista af öllum flugleiðum</t>
+  </si>
+  <si>
+    <t>Yfir 94%  skipuleggjara eiga að geta skráð nýja flugvél í kerfið</t>
+  </si>
+  <si>
+    <t>User group(s)</t>
+  </si>
+  <si>
+    <t>Það þarf að vera hægt að skrá starfsmann með nafni, kennitölu, starfsheiti, heimilsfangi, heimasíma, gsm-síma og netfangi</t>
+  </si>
+  <si>
+    <t>Það þarf að vera hægt að skrá áfangastað með landi, flugvelli, einkennisnúmeri flugvallar, flugtíma, fjarlægð frá Íslandi ásamt nafni tengiliðs og neyðarsímanúmeri</t>
+  </si>
+  <si>
+    <t>Það þarf að vera hægt að skrá vinnuferð með áfangastað, dagsetningu og tíma brottfarar frá Íslandi ásamt dagsetningu og tíma brottfarar til Íslands</t>
+  </si>
+  <si>
+    <t>Það þarf að vera hægt að endurtaka skráningu vinnuferðar fyrir sama áfangastað og tíma yfir á aðra daga</t>
+  </si>
+  <si>
+    <t>Það þarf að vera hægt að breyta upplýsingum um ákveðinn starfsmann að undanskildu nafni og kennitölu</t>
+  </si>
+  <si>
+    <t>Það þarf að vera hægt að sjá lista yfir allar vinnuferðir með flugnúmerum beggja flugferðanna</t>
+  </si>
+  <si>
+    <t>Mannarar eiga að geta skráð nýjan starfmann í 
+kerfið á innan við 2 mínútum að meðaltali</t>
+  </si>
+  <si>
+    <t>Skipuleggjarar eiga að geta skráð nýja vinnuferð í kerfið
+á innan við 2 mínútum að meðaltali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skipuleggjari </t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta birt lista af öllum starfsmönnum
+á innan við 30 sekúndum að meðaltali</t>
+  </si>
+  <si>
     <t>Yfir 94% mannara eiga að breytt upplýsingum um starfsmann
+á innan við 2 mínútum að meðaltali</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta birt lista af öllum flugleiðum
+á innan við 30 sekúndum að meðaltali</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta skráð nýja flugleið í kerfið
+á innan við 2 mínútum að meðaltali</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta skráð nýja flugvél í kerfið
+á innan við 2 mínútum að meðaltali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yfir 94% mannara eiga að geta skráð starfsmenn í vinnuferð </t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta skráð starfsmenn í vinnuferð 
+á innan við 2 mínútum að meðaltali</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta birt lista af starfsmönnum í tiltekinni
+ stöðu</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta birt lista af starfsmönnum í tiltekinni
+ stöðu á innan við 30 sekúndum</t>
+  </si>
+  <si>
+    <t>Yfir 89% starfsmanna eiga að geta birt vinnuferðir eftir dagsetningu</t>
+  </si>
+  <si>
+    <t>Yfir 89% starfsmanna eiga að geta breytt upplýsingum um vinnuferð</t>
+  </si>
+  <si>
+    <t>Skipuleggjari og mannari</t>
+  </si>
+  <si>
+    <t>Yfir 89% starfsmanna eiga að geta birt vinnuferðir eftir dagsetningu
 á innan við 2 mínútum</t>
   </si>
   <si>
-    <t>Yfir 94% skipuleggjara eiga að geta birt lista af öllum flugleiðum</t>
-  </si>
-  <si>
-    <t>Yfir 94% skipuleggjara eiga að geta birt lista af öllum flugleiðum
-á innan við 30 sekúndum</t>
-  </si>
-  <si>
-    <t>Yfir 94%  skipuleggjara eiga að geta skráð nýja flugvél í kerfið</t>
-  </si>
-  <si>
-    <t>Yfir 94%  skipuleggjara eiga að geta skráð nýja flugvél í kerfið
-á innin við 2 mínútum</t>
+    <t>Yfir 89% starfsmanna eiga að geta breytt upplýsingum um vinnuferð
+á innan við 2 mínútum</t>
+  </si>
+  <si>
+    <t>Mannari og
+skipuleggjari</t>
+  </si>
+  <si>
+    <t>Yfir 89% mannara eiga að geta birt starfsmenn sem vinna ekki á
+tilteknum degi</t>
+  </si>
+  <si>
+    <t>Yfir 89% mannara eiga að geta birt starfsmenn sem vinna ekki á
+tilteknum degi á innan við 30 sekúndum</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta birt vikulegu vinnuferðir starfsmanns</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta birt vikulegu vinnuferðir starfsmanns
+á innan við 2 mínútum</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta flett upp réttindi flugmanns til að sjá hvaða vél hann má fljúga</t>
+  </si>
+  <si>
+    <t>Yfir 94% mannara eiga að geta flett upp réttindi flugmanns til að 
+sjá hvaða vél hann má fljúga á innan við 1 mínútu</t>
+  </si>
+  <si>
+    <t>Yfir 89% mannara eiga að geta birt stöðu vinnuferðar</t>
+  </si>
+  <si>
+    <t>Yfir 89% mannara eiga að geta birt stöðu vinnuferðar á innan við
+1 mínútu</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta breytt upplýsingum um tengiliði</t>
+  </si>
+  <si>
+    <t>Yfir 94% skipuleggjara eiga að geta breytt upplýsingum um tengiliði
+á innan við 2 mínútum</t>
+  </si>
+  <si>
+    <t>Effectiveness</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Satisfaction</t>
+  </si>
+  <si>
+    <t>Starfsmenn eiga að gefa meira en 3 í einkunn varðandi ánægju sína
+með kerfið að meðaltali á skalanum 1-5</t>
+  </si>
+  <si>
+    <t>Starfsmenn gefa meira en 3 í einkunn að meðaltali fyrir álits sitt á
+útliti kerfisins á skalanum 1-5 eftir notkun</t>
+  </si>
+  <si>
+    <t>UX</t>
   </si>
 </sst>
 </file>
@@ -806,997 +902,1237 @@
   </sheetPr>
   <dimension ref="B2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="59.44140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="59.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="20"/>
       <c r="C3" s="21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
       <c r="F3" s="24"/>
     </row>
-    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="14">
         <v>1</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B5" s="6">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B6" s="14">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="6">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="14">
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B9" s="6">
         <v>6</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="14">
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="14">
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
         <v>10</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="14">
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="14">
         <v>13</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="2:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="14">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>16</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" s="14">
         <v>17</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="6">
         <v>18</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="14">
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="6">
         <v>20</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="14">
         <v>21</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="6">
         <v>22</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6">
         <v>23</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B27" s="6">
         <v>24</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B28" s="6">
         <v>25</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="6">
         <v>26</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="6">
         <v>27</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" s="6">
         <v>28</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B32" s="6">
         <v>29</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="6">
         <v>30</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="6">
         <v>31</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B35" s="6">
         <v>32</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F35" s="19"/>
     </row>
-    <row r="36" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="6">
         <v>33</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="2:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="6">
         <v>34</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="6">
         <v>35</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B39" s="6">
         <v>36</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F39" s="11"/>
     </row>
-    <row r="40" spans="2:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="6">
         <v>37</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F40" s="11"/>
     </row>
-    <row r="41" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B41" s="6">
         <v>38</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F41" s="11"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B42" s="20"/>
       <c r="C42" s="22" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="23"/>
       <c r="F42" s="24"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43" s="6">
         <v>39</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F43" s="25"/>
-    </row>
-    <row r="44" spans="2:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="6">
         <v>40</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" s="25"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F44" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B45" s="6">
         <v>41</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F45" s="25"/>
-    </row>
-    <row r="46" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="6">
         <v>42</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F46" s="25"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B47" s="6">
         <v>43</v>
       </c>
-      <c r="C47" s="25" t="s">
-        <v>58</v>
+      <c r="C47" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F47" s="25"/>
-    </row>
-    <row r="48" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B48" s="6">
         <v>44</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="25"/>
-    </row>
-    <row r="49" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F48" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B49" s="6">
         <v>45</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>62</v>
+      <c r="C49" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F49" s="25"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B50" s="6">
         <v>46</v>
       </c>
-      <c r="C50" s="25" t="s">
-        <v>60</v>
+      <c r="C50" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F50" s="25"/>
-    </row>
-    <row r="51" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B51" s="6">
         <v>47</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>61</v>
+      <c r="C51" s="25" t="s">
+        <v>52</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F51" s="25"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B52" s="6">
         <v>48</v>
       </c>
-      <c r="C52" s="25" t="s">
-        <v>63</v>
+      <c r="C52" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F52" s="25"/>
-    </row>
-    <row r="53" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B53" s="6">
         <v>49</v>
       </c>
-      <c r="C53" s="7" t="s">
-        <v>64</v>
+      <c r="C53" s="25" t="s">
+        <v>53</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" s="25"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="6">
         <v>50</v>
       </c>
-      <c r="C54" s="25" t="s">
-        <v>65</v>
+      <c r="C54" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F54" s="25"/>
-    </row>
-    <row r="55" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B55" s="6">
         <v>51</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>66</v>
+      <c r="C55" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F55" s="25"/>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B56" s="6">
         <v>52</v>
       </c>
-      <c r="C56" s="25" t="s">
-        <v>67</v>
+      <c r="C56" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F56" s="25"/>
-    </row>
-    <row r="57" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F56" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B57" s="6">
         <v>53</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B58" s="6">
+        <v>54</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D57" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F57" s="25"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B58" s="6"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="25"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B59" s="6"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="25"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B60" s="6"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="25"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="6"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="25"/>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B62" s="6"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="25"/>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B63" s="6"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="25"/>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B64" s="6"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="25"/>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B65" s="6"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="25"/>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B66" s="6"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="25"/>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B67" s="6"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="25"/>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="6"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="25"/>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B69" s="6"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="25"/>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B70" s="6"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="25"/>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B71" s="6"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="25"/>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B72" s="6"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="25"/>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B73" s="6"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="25"/>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B74" s="6"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="25"/>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B75" s="6"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="25"/>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B76" s="6"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="25"/>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B77" s="6"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="25"/>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B78" s="6"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="25"/>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D58" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B59" s="6">
+        <v>55</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B60" s="6">
+        <v>56</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B61" s="6">
+        <v>57</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B62" s="6">
+        <v>58</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B63" s="6">
+        <v>59</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B64" s="6">
+        <v>60</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B65" s="6">
+        <v>61</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B66" s="6">
+        <v>62</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F66" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B67" s="6">
+        <v>63</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B68" s="6">
+        <v>64</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B69" s="6">
+        <v>65</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B70" s="6">
+        <v>66</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B71" s="6">
+        <v>67</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F71" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B72" s="6">
+        <v>68</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D72" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F72" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B73" s="6">
+        <v>69</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F73" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B74" s="6">
+        <v>70</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D74" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F74" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B75" s="6">
+        <v>71</v>
+      </c>
+      <c r="C75" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F75" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B76" s="6">
+        <v>72</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F76" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B77" s="6">
+        <v>73</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D77" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F77" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B78" s="6">
+        <v>74</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D78" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F78" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B79" s="26"/>
       <c r="C79" s="27"/>
       <c r="D79" s="27"/>
@@ -1817,16 +2153,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start on Ui profie display
</commit_message>
<xml_diff>
--- a/documentation/krofulisti.xlsx
+++ b/documentation/krofulisti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patti\Desktop\Verk nám\verklegtnamskeid1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gudmundur\Dropbox\Tölvunarfræði\Verk1\hópverk\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE12FF25-1498-4CF7-A7CE-93856854CC4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D569EAAC-FA3A-457A-83AD-3290321BEF3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-560" yWindow="710" windowWidth="13820" windowHeight="6000" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="kröfur" sheetId="2" r:id="rId1"/>
@@ -902,8 +902,8 @@
   </sheetPr>
   <dimension ref="B2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1531,7 +1531,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F43" s="25" t="s">
         <v>90</v>
@@ -1548,7 +1548,7 @@
         <v>7</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F44" s="25" t="s">
         <v>91</v>
@@ -1565,7 +1565,7 @@
         <v>15</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F45" s="25" t="s">
         <v>90</v>
@@ -1582,7 +1582,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F46" s="25" t="s">
         <v>91</v>
@@ -1599,7 +1599,7 @@
         <v>15</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F47" s="25" t="s">
         <v>90</v>
@@ -1616,7 +1616,7 @@
         <v>15</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F48" s="25" t="s">
         <v>91</v>
@@ -1633,7 +1633,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F49" s="25" t="s">
         <v>90</v>
@@ -1650,7 +1650,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F50" s="25" t="s">
         <v>91</v>
@@ -1667,7 +1667,7 @@
         <v>7</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F51" s="25" t="s">
         <v>90</v>
@@ -1684,7 +1684,7 @@
         <v>7</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F52" s="25" t="s">
         <v>91</v>
@@ -1701,7 +1701,7 @@
         <v>15</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F53" s="25" t="s">
         <v>90</v>
@@ -1718,7 +1718,7 @@
         <v>15</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F54" s="25" t="s">
         <v>91</v>
@@ -1735,7 +1735,7 @@
         <v>15</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F55" s="25" t="s">
         <v>90</v>
@@ -1752,7 +1752,7 @@
         <v>15</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F56" s="25" t="s">
         <v>91</v>
@@ -1769,7 +1769,7 @@
         <v>64</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F57" s="25" t="s">
         <v>90</v>
@@ -1786,7 +1786,7 @@
         <v>15</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F58" s="25" t="s">
         <v>91</v>
@@ -1803,7 +1803,7 @@
         <v>7</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F59" s="25" t="s">
         <v>90</v>
@@ -1820,7 +1820,7 @@
         <v>7</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F60" s="25" t="s">
         <v>91</v>
@@ -1837,7 +1837,7 @@
         <v>7</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F61" s="25" t="s">
         <v>90</v>
@@ -1854,7 +1854,7 @@
         <v>7</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F62" s="25" t="s">
         <v>91</v>
@@ -1871,7 +1871,7 @@
         <v>40</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F63" s="25" t="s">
         <v>90</v>
@@ -1888,7 +1888,7 @@
         <v>40</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F64" s="25" t="s">
         <v>91</v>
@@ -1905,7 +1905,7 @@
         <v>79</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F65" s="25" t="s">
         <v>90</v>
@@ -1922,7 +1922,7 @@
         <v>79</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F66" s="25" t="s">
         <v>91</v>
@@ -1939,7 +1939,7 @@
         <v>7</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F67" s="25" t="s">
         <v>90</v>
@@ -1956,7 +1956,7 @@
         <v>7</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F68" s="25" t="s">
         <v>91</v>
@@ -1973,7 +1973,7 @@
         <v>7</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F69" s="25" t="s">
         <v>90</v>
@@ -1990,7 +1990,7 @@
         <v>7</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F70" s="25" t="s">
         <v>91</v>
@@ -2007,7 +2007,7 @@
         <v>7</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F71" s="25" t="s">
         <v>90</v>
@@ -2024,7 +2024,7 @@
         <v>7</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F72" s="25" t="s">
         <v>91</v>
@@ -2041,7 +2041,7 @@
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F73" s="25" t="s">
         <v>90</v>
@@ -2058,7 +2058,7 @@
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F74" s="25" t="s">
         <v>91</v>
@@ -2075,7 +2075,7 @@
         <v>15</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F75" s="25" t="s">
         <v>90</v>
@@ -2092,7 +2092,7 @@
         <v>15</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F76" s="25" t="s">
         <v>91</v>
@@ -2109,7 +2109,7 @@
         <v>40</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F77" s="25" t="s">
         <v>92</v>
@@ -2126,7 +2126,7 @@
         <v>40</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F78" s="25" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
We no longer have home phone as a requirement
</commit_message>
<xml_diff>
--- a/documentation/krofulisti.xlsx
+++ b/documentation/krofulisti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gudmundur\Dropbox\Tölvunarfræði\Verk1\hópverk\verklegtnamskeid1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D569EAAC-FA3A-457A-83AD-3290321BEF3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D43DB4-296B-44DA-BBE4-6B9974EBCEE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="kröfur" sheetId="2" r:id="rId1"/>
@@ -204,9 +204,6 @@
     <t>User group(s)</t>
   </si>
   <si>
-    <t>Það þarf að vera hægt að skrá starfsmann með nafni, kennitölu, starfsheiti, heimilsfangi, heimasíma, gsm-síma og netfangi</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að skrá áfangastað með landi, flugvelli, einkennisnúmeri flugvallar, flugtíma, fjarlægð frá Íslandi ásamt nafni tengiliðs og neyðarsímanúmeri</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>UX</t>
+  </si>
+  <si>
+    <t>Það þarf að vera hægt að skrá starfsmann með nafni, kennitölu, starfsheiti, heimilsfangi,  gsm-síma og netfangi</t>
   </si>
 </sst>
 </file>
@@ -902,20 +902,20 @@
   </sheetPr>
   <dimension ref="B2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.90625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="59.453125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
@@ -932,7 +932,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="20"/>
       <c r="C3" s="21" t="s">
         <v>36</v>
@@ -941,12 +941,12 @@
       <c r="E3" s="23"/>
       <c r="F3" s="24"/>
     </row>
-    <row r="4" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="14">
         <v>1</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>7</v>
@@ -956,12 +956,12 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>15</v>
@@ -971,12 +971,12 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>15</v>
@@ -986,12 +986,12 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>15</v>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="14">
         <v>5</v>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <v>6</v>
       </c>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>7</v>
       </c>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="6">
         <v>8</v>
       </c>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="14">
         <v>9</v>
       </c>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>10</v>
       </c>
@@ -1091,12 +1091,12 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="14">
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>7</v>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>12</v>
       </c>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="14">
         <v>13</v>
       </c>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="6">
         <v>14</v>
       </c>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="2:6" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14">
         <v>15</v>
       </c>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>16</v>
       </c>
@@ -1174,14 +1174,14 @@
         <v>18</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="14">
         <v>17</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <v>18</v>
       </c>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="14">
         <v>19</v>
       </c>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <v>20</v>
       </c>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="14">
         <v>21</v>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="6">
         <v>22</v>
       </c>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6">
         <v>23</v>
       </c>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <v>24</v>
       </c>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <v>25</v>
       </c>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <v>26</v>
       </c>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>27</v>
       </c>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="6">
         <v>28</v>
       </c>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>29</v>
       </c>
@@ -1376,12 +1376,12 @@
       </c>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="6">
         <v>30</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>40</v>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>31</v>
       </c>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B35" s="6">
         <v>32</v>
       </c>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="F35" s="19"/>
     </row>
-    <row r="36" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
         <v>33</v>
       </c>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="2:6" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="6">
         <v>34</v>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B38" s="6">
         <v>35</v>
       </c>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B39" s="6">
         <v>36</v>
       </c>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="F39" s="11"/>
     </row>
-    <row r="40" spans="2:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="6">
         <v>37</v>
       </c>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="F40" s="11"/>
     </row>
-    <row r="41" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B41" s="6">
         <v>38</v>
       </c>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="F41" s="11"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="20"/>
       <c r="C42" s="22" t="s">
         <v>45</v>
@@ -1520,7 +1520,7 @@
       <c r="E42" s="23"/>
       <c r="F42" s="24"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="6">
         <v>39</v>
       </c>
@@ -1534,15 +1534,15 @@
         <v>23</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="6">
         <v>40</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>7</v>
@@ -1551,10 +1551,10 @@
         <v>39</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="6">
         <v>41</v>
       </c>
@@ -1568,15 +1568,15 @@
         <v>23</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B46" s="6">
         <v>42</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>15</v>
@@ -1585,10 +1585,10 @@
         <v>39</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B47" s="6">
         <v>43</v>
       </c>
@@ -1602,10 +1602,10 @@
         <v>39</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B48" s="6">
         <v>44</v>
       </c>
@@ -1619,10 +1619,10 @@
         <v>39</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="6">
         <v>45</v>
       </c>
@@ -1636,15 +1636,15 @@
         <v>39</v>
       </c>
       <c r="F49" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B50" s="6">
         <v>46</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>7</v>
@@ -1653,10 +1653,10 @@
         <v>39</v>
       </c>
       <c r="F50" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="6">
         <v>47</v>
       </c>
@@ -1670,15 +1670,15 @@
         <v>39</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="6">
         <v>48</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D52" s="25" t="s">
         <v>7</v>
@@ -1687,10 +1687,10 @@
         <v>39</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="6">
         <v>49</v>
       </c>
@@ -1704,15 +1704,15 @@
         <v>39</v>
       </c>
       <c r="F53" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B54" s="6">
         <v>50</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D54" s="25" t="s">
         <v>15</v>
@@ -1721,10 +1721,10 @@
         <v>39</v>
       </c>
       <c r="F54" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="6">
         <v>51</v>
       </c>
@@ -1738,15 +1738,15 @@
         <v>39</v>
       </c>
       <c r="F55" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56" s="6">
         <v>52</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>15</v>
@@ -1755,10 +1755,10 @@
         <v>39</v>
       </c>
       <c r="F56" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="6">
         <v>53</v>
       </c>
@@ -1766,21 +1766,21 @@
         <v>48</v>
       </c>
       <c r="D57" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F57" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58" s="6">
         <v>54</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D58" s="25" t="s">
         <v>15</v>
@@ -1789,15 +1789,15 @@
         <v>39</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="6">
         <v>55</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>7</v>
@@ -1806,15 +1806,15 @@
         <v>39</v>
       </c>
       <c r="F59" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B60" s="6">
         <v>56</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>7</v>
@@ -1823,15 +1823,15 @@
         <v>39</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B61" s="6">
         <v>57</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>7</v>
@@ -1840,15 +1840,15 @@
         <v>39</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="6">
         <v>58</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>7</v>
@@ -1857,15 +1857,15 @@
         <v>39</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="6">
         <v>59</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D63" s="25" t="s">
         <v>40</v>
@@ -1874,15 +1874,15 @@
         <v>39</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B64" s="6">
         <v>60</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D64" s="25" t="s">
         <v>40</v>
@@ -1891,49 +1891,49 @@
         <v>39</v>
       </c>
       <c r="F64" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B65" s="6">
         <v>61</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B66" s="6">
         <v>62</v>
       </c>
       <c r="C66" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="E66" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B67" s="6">
         <v>63</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>7</v>
@@ -1942,15 +1942,15 @@
         <v>39</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B68" s="6">
         <v>64</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>7</v>
@@ -1959,15 +1959,15 @@
         <v>39</v>
       </c>
       <c r="F68" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="6">
         <v>65</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>7</v>
@@ -1976,15 +1976,15 @@
         <v>39</v>
       </c>
       <c r="F69" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B70" s="6">
         <v>66</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>7</v>
@@ -1993,15 +1993,15 @@
         <v>39</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B71" s="6">
         <v>67</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>7</v>
@@ -2010,15 +2010,15 @@
         <v>39</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B72" s="6">
         <v>68</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D72" s="25" t="s">
         <v>7</v>
@@ -2027,15 +2027,15 @@
         <v>39</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="6">
         <v>69</v>
       </c>
       <c r="C73" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D73" s="25" t="s">
         <v>7</v>
@@ -2044,15 +2044,15 @@
         <v>39</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B74" s="6">
         <v>70</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D74" s="25" t="s">
         <v>7</v>
@@ -2061,15 +2061,15 @@
         <v>39</v>
       </c>
       <c r="F74" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="6">
         <v>71</v>
       </c>
       <c r="C75" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D75" s="25" t="s">
         <v>15</v>
@@ -2078,15 +2078,15 @@
         <v>39</v>
       </c>
       <c r="F75" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B76" s="6">
         <v>72</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D76" s="25" t="s">
         <v>15</v>
@@ -2095,15 +2095,15 @@
         <v>39</v>
       </c>
       <c r="F76" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B77" s="6">
         <v>73</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D77" s="25" t="s">
         <v>40</v>
@@ -2112,15 +2112,15 @@
         <v>39</v>
       </c>
       <c r="F77" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B78" s="6">
         <v>74</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D78" s="25" t="s">
         <v>40</v>
@@ -2129,10 +2129,10 @@
         <v>39</v>
       </c>
       <c r="F78" s="25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="26"/>
       <c r="C79" s="27"/>
       <c r="D79" s="27"/>
@@ -2153,14 +2153,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
kröfu og notenda greiningarlistar
</commit_message>
<xml_diff>
--- a/documentation/krofulisti.xlsx
+++ b/documentation/krofulisti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gudmundur\Dropbox\Tölvunarfræði\Verk1\hópverk\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAB9B86-41DF-4E33-B278-3225D12FE629}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C86140A-692B-4A4B-BC64-3B472298EB3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14060" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="kröfur" sheetId="2" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t xml:space="preserve">Name (and possibly a short description) </t>
   </si>
   <si>
-    <t>Additional info</t>
-  </si>
-  <si>
     <t>Priority  (A/B/C)</t>
   </si>
   <si>
@@ -343,13 +340,16 @@
   </si>
   <si>
     <t>Það þarf að vera hægt að skrá starfsmann með nafni, kennitölu, starfsheiti, heimilisfangi,  gsm-síma og netfangi</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +368,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -399,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -476,17 +483,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -496,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -529,12 +525,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -546,14 +536,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -582,6 +566,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -903,19 +893,19 @@
   <dimension ref="B2:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="59.44140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="59.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
@@ -923,1223 +913,1315 @@
         <v>2</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="14">
-        <v>1</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
-        <v>2</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B6" s="14">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F6" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="6">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="14">
+        <v>22</v>
+      </c>
+      <c r="F7" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="12">
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="6">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="12">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B9" s="6">
-        <v>6</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="14">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="14">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="D12" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
         <v>10</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="14">
+      <c r="F13" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="12">
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="12">
         <v>13</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="14">
+      <c r="C16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="D16" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F16" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="2:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14">
+      <c r="F17" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="12">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F18" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>18</v>
+      <c r="C19" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="14">
+      <c r="F19" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="12">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>17</v>
+      <c r="C20" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F20" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="6">
         <v>18</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>38</v>
+      <c r="C21" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="14">
+      <c r="F21" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="12">
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F22" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="6">
         <v>20</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="12">
+        <v>21</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B24" s="14">
-        <v>21</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="D24" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F24" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="6">
         <v>22</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6">
         <v>23</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F26" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B27" s="6">
         <v>24</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F27" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B28" s="6">
         <v>25</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F28" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="6">
         <v>26</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F29" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="6">
         <v>27</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="11"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F30" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" s="6">
         <v>28</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="11"/>
-    </row>
-    <row r="32" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F31" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B32" s="6">
         <v>29</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F32" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="6">
         <v>30</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F33" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="6">
         <v>31</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="11"/>
-    </row>
-    <row r="35" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F34" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B35" s="6">
         <v>32</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F35" s="19"/>
-    </row>
-    <row r="36" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F35" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="6">
         <v>33</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="11"/>
-    </row>
-    <row r="37" spans="2:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F36" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="6">
         <v>34</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="11"/>
-    </row>
-    <row r="38" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F37" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="6">
         <v>35</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="11"/>
-    </row>
-    <row r="39" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F38" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B39" s="6">
         <v>36</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="11"/>
-    </row>
-    <row r="40" spans="2:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F39" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="6">
         <v>37</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D40" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B41" s="6">
+        <v>38</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F40" s="11"/>
-    </row>
-    <row r="41" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B41" s="6">
-        <v>38</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="D41" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F41" s="11"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="20"/>
-      <c r="C42" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F41" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="16"/>
+      <c r="C42" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43" s="6">
         <v>39</v>
       </c>
-      <c r="C43" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>7</v>
+      <c r="C43" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="6">
         <v>40</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>7</v>
+        <v>60</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F44" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B45" s="6">
         <v>41</v>
       </c>
-      <c r="C45" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>15</v>
+      <c r="C45" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F45" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="6">
         <v>42</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>15</v>
+        <v>61</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F46" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B47" s="6">
         <v>43</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="25" t="s">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F47" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B48" s="6">
         <v>44</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>15</v>
+        <v>50</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F48" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B49" s="6">
         <v>45</v>
       </c>
-      <c r="C49" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>7</v>
+      <c r="C49" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F49" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B50" s="6">
         <v>46</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>7</v>
+        <v>63</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F50" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B51" s="6">
         <v>47</v>
       </c>
-      <c r="C51" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>7</v>
+      <c r="C51" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F51" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B52" s="6">
         <v>48</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>7</v>
+        <v>64</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F52" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B53" s="6">
         <v>49</v>
       </c>
-      <c r="C53" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>15</v>
+      <c r="C53" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F53" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="6">
         <v>50</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>15</v>
+        <v>65</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F54" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B55" s="6">
         <v>51</v>
       </c>
-      <c r="C55" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>15</v>
+      <c r="C55" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F55" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B56" s="6">
         <v>52</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>15</v>
+        <v>67</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F56" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B57" s="6">
         <v>53</v>
       </c>
-      <c r="C57" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>63</v>
+      <c r="C57" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F57" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B58" s="6">
         <v>54</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>15</v>
+        <v>66</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F58" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B59" s="6">
         <v>55</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>7</v>
+        <v>68</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F59" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B60" s="6">
         <v>56</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>7</v>
+        <v>69</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F60" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B61" s="6">
         <v>57</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D61" s="25" t="s">
-        <v>7</v>
+        <v>70</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F61" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B62" s="6">
         <v>58</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D62" s="25" t="s">
-        <v>7</v>
+        <v>71</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F62" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B63" s="6">
         <v>59</v>
       </c>
-      <c r="C63" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D63" s="25" t="s">
-        <v>40</v>
+      <c r="C63" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>39</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F63" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F63" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B64" s="6">
         <v>60</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D64" s="25" t="s">
-        <v>40</v>
+        <v>75</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>39</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F64" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B65" s="6">
         <v>61</v>
       </c>
-      <c r="C65" s="25" t="s">
-        <v>74</v>
+      <c r="C65" s="21" t="s">
+        <v>73</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F65" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B66" s="6">
         <v>62</v>
       </c>
       <c r="C66" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="E66" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F66" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B67" s="6">
         <v>63</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D67" s="25" t="s">
-        <v>7</v>
+        <v>78</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F67" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F67" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B68" s="6">
         <v>64</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D68" s="25" t="s">
-        <v>7</v>
+        <v>79</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F68" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B69" s="6">
         <v>65</v>
       </c>
-      <c r="C69" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D69" s="25" t="s">
-        <v>7</v>
+      <c r="C69" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F69" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B70" s="6">
         <v>66</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D70" s="25" t="s">
-        <v>7</v>
+        <v>81</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F70" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F70" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B71" s="6">
         <v>67</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D71" s="25" t="s">
-        <v>7</v>
+        <v>82</v>
+      </c>
+      <c r="D71" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F71" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B72" s="6">
         <v>68</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D72" s="25" t="s">
-        <v>7</v>
+        <v>83</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F72" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B73" s="6">
         <v>69</v>
       </c>
-      <c r="C73" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="D73" s="25" t="s">
-        <v>7</v>
+      <c r="C73" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F73" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B74" s="6">
         <v>70</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D74" s="25" t="s">
-        <v>7</v>
+        <v>85</v>
+      </c>
+      <c r="D74" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F74" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F74" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B75" s="6">
         <v>71</v>
       </c>
-      <c r="C75" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D75" s="25" t="s">
-        <v>15</v>
+      <c r="C75" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D75" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F75" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F75" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B76" s="6">
         <v>72</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D76" s="25" t="s">
-        <v>15</v>
+        <v>87</v>
+      </c>
+      <c r="D76" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F76" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F76" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B77" s="6">
         <v>73</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D77" s="25" t="s">
-        <v>40</v>
+        <v>91</v>
+      </c>
+      <c r="D77" s="21" t="s">
+        <v>39</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F77" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F77" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B78" s="6">
         <v>74</v>
       </c>
       <c r="C78" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D78" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F78" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D78" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F78" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="26"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="28"/>
-      <c r="F79" s="29"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B79" s="22"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="25"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F4:F41">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -2153,16 +2235,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>